<commit_message>
added ModelBAS.mwb - log model db, edited docs
</commit_message>
<xml_diff>
--- a/documets/Структура и содержание базы данных/table_info.xlsx
+++ b/documets/Структура и содержание базы данных/table_info.xlsx
@@ -1,38 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivira\OneDrive\Рабочий стол\Дистанционка\Табунов\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\basystem\BankAssistanceSystem\documets\Структура и содержание базы данных\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD1F0CA-1CDB-40B2-A2FE-38F82D4554DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3449BDF2-790F-4F28-9D90-A7731604CA28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" firstSheet="4" activeTab="7" xr2:uid="{A3D8686D-AE4A-4D86-A985-D42EA9E9F4DA}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{A3D8686D-AE4A-4D86-A985-D42EA9E9F4DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
     <sheet name="BANK_USER" sheetId="2" r:id="rId2"/>
-    <sheet name="BANK_USER_ACCESS" sheetId="3" r:id="rId3"/>
-    <sheet name="BANK_USER_STATUS" sheetId="4" r:id="rId4"/>
-    <sheet name="BANK_CURRENCY" sheetId="11" r:id="rId5"/>
-    <sheet name="BANK_CLIENT" sheetId="23" r:id="rId6"/>
-    <sheet name="BANK_ACTIVE_AUTHORIZED_CAPITAL" sheetId="5" r:id="rId7"/>
-    <sheet name="BANK_PASSIVE_AUTHORIZED_CAPITAL" sheetId="6" r:id="rId8"/>
-    <sheet name="BANK_ACTIVE_CAMP" sheetId="7" r:id="rId9"/>
-    <sheet name="BANK_PASSIVE_CAMP" sheetId="8" r:id="rId10"/>
-    <sheet name="BANK_PASSIVE_ADD_CAPITAL" sheetId="9" r:id="rId11"/>
-    <sheet name="BANK_ACTIVE_CREDITS_OUT" sheetId="18" r:id="rId12"/>
-    <sheet name="BANK_ACTIVE_DOCS" sheetId="10" r:id="rId13"/>
-    <sheet name="BANK_PASSIVE_CORRES_ACCOUTS" sheetId="19" r:id="rId14"/>
-    <sheet name="BANK_PASSIVE_DEPOSITS" sheetId="20" r:id="rId15"/>
-    <sheet name="BANK_ACTIVE_DEPOSITS" sheetId="21" r:id="rId16"/>
-    <sheet name="BANK_PASSIVE_CREDIT_DEBIT" sheetId="22" r:id="rId17"/>
-    <sheet name="BANK_ACTIVE_ASSET" sheetId="24" r:id="rId18"/>
-    <sheet name="BANK_ACTIVE_CLIENT_ASSET" sheetId="25" r:id="rId19"/>
-    <sheet name="BANK_ACTIVE_DEBIT" sheetId="31" r:id="rId20"/>
+    <sheet name="BANK_CLIENT_HISTORY" sheetId="33" r:id="rId3"/>
+    <sheet name="BANK_USER_ACCESS" sheetId="3" r:id="rId4"/>
+    <sheet name="BANK_USER_STATUS" sheetId="4" r:id="rId5"/>
+    <sheet name="BANK_CURRENCY" sheetId="11" r:id="rId6"/>
+    <sheet name="BANK_CLIENT" sheetId="23" r:id="rId7"/>
+    <sheet name="BANK_CLIENT_COMPANY" sheetId="32" r:id="rId8"/>
+    <sheet name="BANK_ACTIVE_AUTHORIZED_CAPITAL" sheetId="5" r:id="rId9"/>
+    <sheet name="BANK_PASSIVE_AUTHORIZED_CAPITAL" sheetId="6" r:id="rId10"/>
+    <sheet name="BANK_ACTIVE_CAMP" sheetId="7" r:id="rId11"/>
+    <sheet name="BANK_PASSIVE_CAMP" sheetId="8" r:id="rId12"/>
+    <sheet name="BANK_PASSIVE_ADD_CAPITAL" sheetId="9" r:id="rId13"/>
+    <sheet name="BANK_ACTIVE_CREDITS_OUT" sheetId="18" r:id="rId14"/>
+    <sheet name="BANK_ACTIVE_DOCS" sheetId="10" r:id="rId15"/>
+    <sheet name="BANK_PASSIVE_CORRES_ACCOUTS" sheetId="19" r:id="rId16"/>
+    <sheet name="BANK_PASSIVE_DEPOSITS" sheetId="20" r:id="rId17"/>
+    <sheet name="BANK_ACTIVE_DEPOSITS" sheetId="21" r:id="rId18"/>
+    <sheet name="BANK_PASSIVE_CREDIT_DEBIT" sheetId="22" r:id="rId19"/>
+    <sheet name="BANK_ACTIVE_ASSET" sheetId="24" r:id="rId20"/>
+    <sheet name="BANK_ACTIVE_CLIENT_ASSET" sheetId="25" r:id="rId21"/>
+    <sheet name="BANK_ACTIVE_DEBIT" sheetId="31" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="203">
   <si>
     <t>NAME</t>
   </si>
@@ -391,12 +393,6 @@
     <t>Корреспондентские счета коммерческих банков, открытые в банке</t>
   </si>
   <si>
-    <t>Кому заняли (банк)</t>
-  </si>
-  <si>
-    <t>ca_bank_debtor</t>
-  </si>
-  <si>
     <t>ca_bank_name</t>
   </si>
   <si>
@@ -547,9 +543,6 @@
     <t xml:space="preserve">cass_id </t>
   </si>
   <si>
-    <t>cass_debtor</t>
-  </si>
-  <si>
     <t>cass_cash</t>
   </si>
   <si>
@@ -578,6 +571,90 @@
   </si>
   <si>
     <t>Тип средства(золото, Руб. Дол.)</t>
+  </si>
+  <si>
+    <t>BANK_CLIENT_COMPANY</t>
+  </si>
+  <si>
+    <t>Информация об компании клиента</t>
+  </si>
+  <si>
+    <t>cl_comp_id</t>
+  </si>
+  <si>
+    <t>cl_comp_name</t>
+  </si>
+  <si>
+    <t>cl_comp_descr</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>act_deposit_type</t>
+  </si>
+  <si>
+    <t>cass_client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Уставной капитал банка </t>
+  </si>
+  <si>
+    <t>У кого счет</t>
+  </si>
+  <si>
+    <t>ca_bank_company</t>
+  </si>
+  <si>
+    <t>BANK_CLIENT_HISTORY</t>
+  </si>
+  <si>
+    <t>Иформация кредитов слиента</t>
+  </si>
+  <si>
+    <t>clihis_id</t>
+  </si>
+  <si>
+    <t>clihi_numb</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>clihis_start_date</t>
+  </si>
+  <si>
+    <t>clihis_client</t>
+  </si>
+  <si>
+    <t>clihis_all_sum</t>
+  </si>
+  <si>
+    <t>clihis_paid_off</t>
+  </si>
+  <si>
+    <t>clihis_paid</t>
+  </si>
+  <si>
+    <t>clihis_status</t>
+  </si>
+  <si>
+    <t>clihis_percent</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>clihis_ddl_date</t>
+  </si>
+  <si>
+    <t>clihis_tdl_date</t>
   </si>
 </sst>
 </file>
@@ -593,22 +670,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -624,13 +686,32 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -645,22 +726,23 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -973,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACAC0E98-1FA9-4D9E-8497-CEC1F9700000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,7 +1069,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
@@ -995,7 +1077,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1003,7 +1085,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
@@ -1011,7 +1093,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B4" t="s">
@@ -1019,160 +1101,280 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>143</v>
+      <c r="A5" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B14" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" t="s">
-        <v>135</v>
-      </c>
-    </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="BANK_USER!A1" display="BANK_USER" xr:uid="{3E4D99DB-9552-4A6C-AA8B-3D5B23AB6070}"/>
     <hyperlink ref="A2" location="BANK_USER_ACCESS!A1" display="BANK_USER_ACCESS" xr:uid="{CBC6C8D9-1953-426B-84F2-E9CD5038A084}"/>
     <hyperlink ref="A3" location="BANK_USER_STATUS!A1" display="BANK_USER_STATUS" xr:uid="{ACDEBE46-B1C4-4AD8-B469-45DFA09D34AE}"/>
-    <hyperlink ref="A6" location="BANK_ACTIVE_AUTHORIZED_CAPITAL!A1" display="BANK_ACTIVE_AUTHORIZED_CAPITAL" xr:uid="{B6851E03-4D78-4FFA-B76E-35887834C7AA}"/>
-    <hyperlink ref="A14" location="BANK_PASSIVE_AUTHORIZED_CAPITAL!A1" display="BANK_PASSIVE_AUTHORIZED_CAPITAL" xr:uid="{1D89AAC8-EB8F-44AB-B3F6-B4C30ED12468}"/>
-    <hyperlink ref="A7" location="BANK_ACTIVE_CAMP!A1" display="BANK_ACTIVE_CAMP" xr:uid="{640AFCBC-CF46-444B-9CB1-4763179EEB7F}"/>
-    <hyperlink ref="A15" location="BANK_PASSIVE_CAMP!A1" display="BANK_PASSIVE_CAMP" xr:uid="{9F453C31-5E34-4127-A64E-3974468F22A3}"/>
-    <hyperlink ref="A16" location="BANK_PASSIVE_ADD_CAPITAL!A1" display="BANK_PASSIVE_ADD_CAPITAL" xr:uid="{6D64C52B-4AA6-41E3-BB13-8ECEB86B2753}"/>
+    <hyperlink ref="A8" location="BANK_ACTIVE_AUTHORIZED_CAPITAL!A1" display="BANK_ACTIVE_AUTHORIZED_CAPITAL" xr:uid="{B6851E03-4D78-4FFA-B76E-35887834C7AA}"/>
+    <hyperlink ref="A16" location="BANK_PASSIVE_AUTHORIZED_CAPITAL!A1" display="BANK_PASSIVE_AUTHORIZED_CAPITAL" xr:uid="{1D89AAC8-EB8F-44AB-B3F6-B4C30ED12468}"/>
+    <hyperlink ref="A9" location="BANK_ACTIVE_CAMP!A1" display="BANK_ACTIVE_CAMP" xr:uid="{640AFCBC-CF46-444B-9CB1-4763179EEB7F}"/>
+    <hyperlink ref="A17" location="BANK_PASSIVE_CAMP!A1" display="BANK_PASSIVE_CAMP" xr:uid="{9F453C31-5E34-4127-A64E-3974468F22A3}"/>
+    <hyperlink ref="A18" location="BANK_PASSIVE_ADD_CAPITAL!A1" display="BANK_PASSIVE_ADD_CAPITAL" xr:uid="{6D64C52B-4AA6-41E3-BB13-8ECEB86B2753}"/>
     <hyperlink ref="A4" location="BANK_CURRENCY!A1" display="BANK_CURRENCY" xr:uid="{C53C5276-2E9F-4695-8427-CC1316844D4C}"/>
-    <hyperlink ref="A8" location="BANK_ACTIVE_DOCS!A1" display="BANK_ACTIVE_DOCS" xr:uid="{79631A27-F374-4CE9-AF75-96099685CDAB}"/>
-    <hyperlink ref="A9" location="BANK_ACTIVE_CREDITS_OUT!A1" display="BANK_ACTIVE_CREDITS_OUT" xr:uid="{A5614DA8-9735-48E1-B4F1-AB648F9F06BD}"/>
-    <hyperlink ref="A17" location="BANK_PASSIVE_CORRES_ACCOUTS!A1" display="BANK_PASSIVE_CORRES_ACCOUTS" xr:uid="{FCA24A6B-D76D-40AB-BBEE-3A78F6B44FF9}"/>
-    <hyperlink ref="A18" location="BANK_PASSIVE_DEPOSITS!A1" display="BANK_PASSIVE_DEPOSITS" xr:uid="{8EA05233-5295-4951-833B-3AB7090EF641}"/>
-    <hyperlink ref="A10" location="BANK_ACTIVE_DOCS!A1" display="BANK_ACTIVE_DOCS" xr:uid="{FDE770A1-C4B5-45E3-8610-DBE551F9087F}"/>
-    <hyperlink ref="A19" location="BANK_PASSIVE_CREDIT_DEBIT!A1" display="BANK_PASSIVE_CREDIT_DEBIT" xr:uid="{EE577FA0-E898-45D4-816D-5E69034525C6}"/>
+    <hyperlink ref="A10" location="BANK_ACTIVE_DOCS!A1" display="BANK_ACTIVE_DOCS" xr:uid="{79631A27-F374-4CE9-AF75-96099685CDAB}"/>
+    <hyperlink ref="A11" location="BANK_ACTIVE_CREDITS_OUT!A1" display="BANK_ACTIVE_CREDITS_OUT" xr:uid="{A5614DA8-9735-48E1-B4F1-AB648F9F06BD}"/>
+    <hyperlink ref="A19" location="BANK_PASSIVE_CORRES_ACCOUTS!A1" display="BANK_PASSIVE_CORRES_ACCOUTS" xr:uid="{FCA24A6B-D76D-40AB-BBEE-3A78F6B44FF9}"/>
+    <hyperlink ref="A20" location="BANK_PASSIVE_DEPOSITS!A1" display="BANK_PASSIVE_DEPOSITS" xr:uid="{8EA05233-5295-4951-833B-3AB7090EF641}"/>
+    <hyperlink ref="A12" location="BANK_ACTIVE_DEPOSITS!A1" display="BANK_ACTIVE_DEPOSITS" xr:uid="{FDE770A1-C4B5-45E3-8610-DBE551F9087F}"/>
+    <hyperlink ref="A21" location="BANK_PASSIVE_CREDIT_DEBIT!A1" display="BANK_PASSIVE_CREDIT_DEBIT" xr:uid="{EE577FA0-E898-45D4-816D-5E69034525C6}"/>
     <hyperlink ref="A5" location="BANK_CLIENT!A1" display="BANK_CLIENT" xr:uid="{EA994D3E-D24D-45A4-B618-57BD71C808EB}"/>
-    <hyperlink ref="A11" location="BANK_ACTIVE_ASSET!A1" display="BANK_ACTIVE_ASSET" xr:uid="{8CE45541-C8C6-4075-89F7-1521B5E6BAAD}"/>
-    <hyperlink ref="A12" location="BANK_ACTIVE_CLIENT_ASSET!A1" display="BANK_ACTIVE_CLIENT_ASSET" xr:uid="{D1A0FBB1-A461-4ACA-8D9D-E343D6EB799F}"/>
-    <hyperlink ref="A13" location="BANK_ACTIVE_DEBIT!A1" display="BANK_ACTIVE_DEBIT" xr:uid="{B44BF314-872C-449D-8F06-BFCD6CDA5888}"/>
+    <hyperlink ref="A13" location="BANK_ACTIVE_ASSET!A1" display="BANK_ACTIVE_ASSET" xr:uid="{8CE45541-C8C6-4075-89F7-1521B5E6BAAD}"/>
+    <hyperlink ref="A14" location="BANK_ACTIVE_CLIENT_ASSET!A1" display="BANK_ACTIVE_CLIENT_ASSET" xr:uid="{D1A0FBB1-A461-4ACA-8D9D-E343D6EB799F}"/>
+    <hyperlink ref="A15" location="BANK_ACTIVE_DEBIT!A1" display="BANK_ACTIVE_DEBIT" xr:uid="{B44BF314-872C-449D-8F06-BFCD6CDA5888}"/>
+    <hyperlink ref="A7" location="BANK_CLIENT_HISTORY!A1" display="BANK_CLIENT_HISTORY" xr:uid="{A0947CA0-EE2E-4856-8986-F4C7B882EE54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B51AE-AE70-4733-A0D6-5BA4F9139A7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31ACC511-8A91-4465-9B33-463B07812C5C}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{34669BF1-2C3E-4937-8C0A-1DD493B67A14}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF49509-33B7-4AD4-83CA-D6E2533A00FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1400,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1209,7 +1411,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -1223,7 +1425,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
@@ -1234,9 +1436,9 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D5" t="s">
@@ -1245,18 +1447,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{025CC5D1-AE4F-45C3-937F-2E65ED57E2A5}"/>
+    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{A350E3F2-38EE-44FF-BB65-6FEE0721FF47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD1AB63-D7D0-4E52-96D2-79191696CCB1}">
-  <dimension ref="A1:D7"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B51AE-AE70-4733-A0D6-5BA4F9139A7C}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1484,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1293,73 +1495,54 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
+      <c r="C3">
+        <v>250</v>
+      </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" t="s">
-        <v>177</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{CFF15DC4-4593-4658-BDFB-7EF476F8929B}"/>
+    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{025CC5D1-AE4F-45C3-937F-2E65ED57E2A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003407C2-7CAD-498D-944F-7A81FC78221A}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD1AB63-D7D0-4E52-96D2-79191696CCB1}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,7 +1568,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1396,74 +1579,73 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>79</v>
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{F48FA222-4E99-459D-9C18-820E408BCF56}"/>
-    <hyperlink ref="B5" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{D9668447-BCFE-4DD2-BE4A-21C9923308FF}"/>
+    <hyperlink ref="B7" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{CFF15DC4-4593-4658-BDFB-7EF476F8929B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD95C3F7-367D-470D-9821-2B30323D984C}">
-  <dimension ref="A1:D6"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003407C2-7CAD-498D-944F-7A81FC78221A}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,7 +1671,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1500,406 +1682,71 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
+        <v>110</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{07555C08-295E-4A4C-8AC4-747364282E6F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14B3B7F-BC12-4061-BE92-B7D0AD1267A0}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="52.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{B05177EF-D1D9-4052-9ECC-21A78BCC0358}"/>
-    <hyperlink ref="B4" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{7FFEBFC0-DAB2-4523-8531-339EA956024B}"/>
+    <hyperlink ref="B7" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{F48FA222-4E99-459D-9C18-820E408BCF56}"/>
+    <hyperlink ref="B5" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{D9668447-BCFE-4DD2-BE4A-21C9923308FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1609D026-E675-44B6-8737-818E774DA10E}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="52.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{6EE0F6EF-D883-40FC-8D57-F25FB8BB94E3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5978044B-7B7A-451F-BD66-0BA6A6D293EE}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="52.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{2B4563EB-DD95-490B-9A49-73A8FBA25336}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C6B8A6-1CD0-4F87-BD61-1F00BFE2BC4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD95C3F7-367D-470D-9821-2B30323D984C}">
   <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="52.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{A780604A-4180-4432-B72B-ABAE3538DA1F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D156B587-93A3-4A52-8E09-5310E9B7F915}">
-  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1926,7 +1773,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1937,51 +1784,62 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{1E4A3E49-76A6-43B8-8B3A-25F0C73B898B}"/>
+    <hyperlink ref="B6" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{07555C08-295E-4A4C-8AC4-747364282E6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCB98DB-2F24-4E11-B31E-F34583F0DEAE}">
-  <dimension ref="A1:D5"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14B3B7F-BC12-4061-BE92-B7D0AD1267A0}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2007,7 +1865,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2018,187 +1876,63 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+        <v>185</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{0D76F371-E31C-40C8-9811-950BBB77FAE9}"/>
-    <hyperlink ref="B3" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{7206C2D3-3E83-4A93-A120-53DDD39E9D9D}"/>
+    <hyperlink ref="B6" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{B05177EF-D1D9-4052-9ECC-21A78BCC0358}"/>
+    <hyperlink ref="B4" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{7FFEBFC0-DAB2-4523-8531-339EA956024B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD51FA2-D2D6-4566-B428-7C1E6F818FAC}">
-  <dimension ref="A1:D10"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1609D026-E675-44B6-8737-818E774DA10E}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="10" width="17.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B9" location="BANK_USER_STATUS!A2:D2" display="int" xr:uid="{69B83BA9-0CF8-4439-B8FD-78567D202BDE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F6CD24-3158-4EEB-A718-DB2648E89761}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2224,7 +1958,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2235,42 +1969,594 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{6EE0F6EF-D883-40FC-8D57-F25FB8BB94E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5978044B-7B7A-451F-BD66-0BA6A6D293EE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{2B4563EB-DD95-490B-9A49-73A8FBA25336}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C6B8A6-1CD0-4F87-BD61-1F00BFE2BC4F}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>139</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{A780604A-4180-4432-B72B-ABAE3538DA1F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD51FA2-D2D6-4566-B428-7C1E6F818FAC}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="10" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" location="BANK_USER_STATUS!A2:D2" display="int" xr:uid="{69B83BA9-0CF8-4439-B8FD-78567D202BDE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D156B587-93A3-4A52-8E09-5310E9B7F915}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{1E4A3E49-76A6-43B8-8B3A-25F0C73B898B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCB98DB-2F24-4E11-B31E-F34583F0DEAE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{0D76F371-E31C-40C8-9811-950BBB77FAE9}"/>
+    <hyperlink ref="B3" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{7206C2D3-3E83-4A93-A120-53DDD39E9D9D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F6CD24-3158-4EEB-A718-DB2648E89761}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D6" t="s">
@@ -2286,11 +2572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9508FB1E-D243-4E2A-91AF-16476DCA7BA4}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06016087-ED14-4C2E-A010-63A4AD8F429D}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2316,6 +2602,135 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" location="BANK_CLIENT!A1" display="int foreign key" xr:uid="{E9BB8490-A6DB-4358-B991-4D0ED03A9D8E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9508FB1E-D243-4E2A-91AF-16476DCA7BA4}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
@@ -2329,7 +2744,7 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D3" t="s">
@@ -2369,12 +2784,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8316E026-C455-4FAF-9FE7-00C88C449B0A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2439,13 +2854,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD05B0B9-FABE-4C74-A22B-FBDC8536F6FC}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2497,7 +2910,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2508,7 +2921,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2517,7 +2930,7 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2528,12 +2941,147 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECDE5D9A-52FD-4A44-84DB-36C1F41BC3A8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9F97B9-4CB9-4947-BB34-6A6DF0CDC04A}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2559,7 +3107,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2570,7 +3118,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -2579,12 +3127,12 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -2593,71 +3141,7 @@
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7">
-        <v>150</v>
-      </c>
-      <c r="D7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2665,12 +3149,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87BB855-52C1-43EB-8FD6-8B8E1F271739}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2756,7 +3240,7 @@
       <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
@@ -2769,192 +3253,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31ACC511-8A91-4465-9B33-463B07812C5C}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3">
-        <v>500</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{34669BF1-2C3E-4937-8C0A-1DD493B67A14}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF49509-33B7-4AD4-83CA-D6E2533A00FB}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="52.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3">
-        <v>250</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" location="BANK_CURRENCY!A1" display="int foreign key" xr:uid="{A350E3F2-38EE-44FF-BB65-6FEE0721FF47}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
mod style, js, html and docs
</commit_message>
<xml_diff>
--- a/documets/Структура и содержание базы данных/table_info.xlsx
+++ b/documets/Структура и содержание базы данных/table_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\basystem\BankAssistanceSystem\documets\Структура и содержание базы данных\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3449BDF2-790F-4F28-9D90-A7731604CA28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146FBA97-67A6-4FB6-A5CE-A33245EDD761}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{A3D8686D-AE4A-4D86-A985-D42EA9E9F4DA}"/>
+    <workbookView xWindow="-6612" yWindow="4884" windowWidth="17280" windowHeight="9072" xr2:uid="{A3D8686D-AE4A-4D86-A985-D42EA9E9F4DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="205">
   <si>
     <t>NAME</t>
   </si>
@@ -447,9 +447,6 @@
     <t>pas_deposit_cash</t>
   </si>
   <si>
-    <t>Кредиторская задолженность</t>
-  </si>
-  <si>
     <t>BANK_PASSIVE_CREDIT_DEBIT</t>
   </si>
   <si>
@@ -609,9 +606,6 @@
     <t>BANK_CLIENT_HISTORY</t>
   </si>
   <si>
-    <t>Иформация кредитов слиента</t>
-  </si>
-  <si>
     <t>clihis_id</t>
   </si>
   <si>
@@ -655,6 +649,18 @@
   </si>
   <si>
     <t>clihis_tdl_date</t>
+  </si>
+  <si>
+    <t>addc_debit</t>
+  </si>
+  <si>
+    <t>addc_credit</t>
+  </si>
+  <si>
+    <t>addc_type</t>
+  </si>
+  <si>
+    <t>Иформация кредитов клиента</t>
   </si>
 </sst>
 </file>
@@ -733,12 +739,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1057,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACAC0E98-1FA9-4D9E-8497-CEC1F9700000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,7 +1075,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
@@ -1077,7 +1083,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1085,7 +1091,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
@@ -1093,7 +1099,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B4" t="s">
@@ -1101,31 +1107,31 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>141</v>
+      <c r="A5" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
         <v>175</v>
       </c>
-      <c r="B6" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>186</v>
+      <c r="A7" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B8" t="s">
@@ -1133,7 +1139,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B9" t="s">
@@ -1141,7 +1147,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B10" t="s">
@@ -1149,7 +1155,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B11" t="s">
@@ -1157,7 +1163,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B12" t="s">
@@ -1165,39 +1171,39 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>152</v>
+      <c r="A13" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>158</v>
+      <c r="A14" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>170</v>
+      <c r="A15" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B17" t="s">
@@ -1205,7 +1211,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B18" t="s">
@@ -1213,7 +1219,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B19" t="s">
@@ -1221,7 +1227,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B20" t="s">
@@ -1229,11 +1235,11 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>134</v>
+      <c r="A21" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1548,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,7 +1607,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -1612,7 +1618,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -1623,13 +1629,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>203</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1748,7 +1754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD95C3F7-367D-470D-9821-2B30323D984C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1887,13 +1895,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1991,7 +1999,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>79</v>
@@ -2072,7 +2080,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>79</v>
@@ -2120,7 +2128,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2131,7 +2139,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -2142,18 +2150,18 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -2164,7 +2172,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>79</v>
@@ -2211,7 +2219,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2347,7 +2355,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2358,29 +2366,29 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>79</v>
@@ -2428,7 +2436,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2439,29 +2447,29 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>79</v>
@@ -2510,7 +2518,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2521,7 +2529,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -2532,29 +2540,29 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>79</v>
@@ -2575,8 +2583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06016087-ED14-4C2E-A010-63A4AD8F429D}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2602,7 +2610,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2613,15 +2621,15 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>79</v>
@@ -2629,24 +2637,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -2654,15 +2662,15 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -2670,7 +2678,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -2678,7 +2686,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -2686,10 +2694,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2705,7 +2713,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2910,7 +2918,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2921,7 +2929,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2930,7 +2938,7 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2970,7 +2978,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2981,7 +2989,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -2995,7 +3003,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -3009,7 +3017,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
@@ -3023,18 +3031,18 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -3043,12 +3051,12 @@
         <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -3062,7 +3070,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3107,7 +3115,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -3118,7 +3126,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -3127,12 +3135,12 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>

</xml_diff>